<commit_message>
update code call api giam gia sp theo boi so
</commit_message>
<xml_diff>
--- a/src/main/resources/HTGiamGiaSPTheoBoiSo.xlsx
+++ b/src/main/resources/HTGiamGiaSPTheoBoiSo.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThuPhuoc\MyAutomation\finviet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE0D0DD-1178-4B91-9732-632B25EDE5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA2C8C7-C4B0-4668-9200-84B259FC6DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="12240" tabRatio="580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ThongTinCoBanKM" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="195">
   <si>
     <t>Kênh mua hàng</t>
   </si>
@@ -631,7 +631,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -977,6 +976,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,12 +989,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1411,20 +1410,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="13.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="24.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="26.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="10.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="7.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="12.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="12.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="17.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="17.109375" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="13.21875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1514,48 +1513,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AS147"/>
+  <dimension ref="A1:AT147"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
       <selection activeCell="BG2" sqref="BG2"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+      <selection pane="topRight" activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="19" width="4.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="15" width="13.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="16" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="16" width="13.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="8" width="17.77734375" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" style="15" width="19.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="15" width="31.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="16" width="21.77734375" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="16" width="18.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="17" width="25.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="17" width="18.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="17" width="35.44140625" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="18" max="20" customWidth="true" style="15" width="17.0" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="24" max="26" customWidth="true" style="15" width="17.0" collapsed="true"/>
-    <col min="27" max="29" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="30" max="32" customWidth="true" style="37" width="16.88671875" collapsed="true"/>
-    <col min="33" max="34" customWidth="true" style="37" width="15.109375" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" style="37" width="16.21875" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" style="19" width="32.6640625" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="19" width="19.21875" collapsed="true"/>
-    <col min="38" max="38" customWidth="true" style="19" width="37.77734375" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="19" width="24.77734375" collapsed="true"/>
-    <col min="40" max="42" customWidth="true" style="19" width="19.21875" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" style="19" width="25.77734375" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" style="14" width="35.5546875" collapsed="true"/>
-    <col min="45" max="45" customWidth="true" style="14" width="23.88671875" collapsed="true"/>
-    <col min="46" max="16384" style="14" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="4.33203125" style="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.77734375" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.77734375" style="8" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="19.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="18.21875" style="16" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25" style="17" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="35.44140625" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="18" max="20" width="17" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="24" max="26" width="17" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="29" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="30" max="32" width="16.88671875" style="37" customWidth="1" collapsed="1"/>
+    <col min="33" max="34" width="15.109375" style="37" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="16.21875" style="37" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="32.6640625" style="19" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="19.21875" style="19" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="25.77734375" style="19" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="37.77734375" style="19" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="24.77734375" style="19" customWidth="1" collapsed="1"/>
+    <col min="41" max="43" width="19.21875" style="19" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="25.77734375" style="19" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="35.5546875" style="14" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="23.88671875" style="14" customWidth="1" collapsed="1"/>
+    <col min="47" max="16384" width="8.88671875" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="36" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" s="36" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>69</v>
       </c>
@@ -1668,31 +1668,34 @@
         <v>63</v>
       </c>
       <c r="AL1" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM1" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="AM1" s="29" t="s">
+      <c r="AN1" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="AN1" s="29" t="s">
+      <c r="AO1" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="AO1" s="29" t="s">
+      <c r="AP1" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="AP1" s="29" t="s">
+      <c r="AQ1" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="AQ1" s="29" t="s">
+      <c r="AR1" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AR1" s="36" t="s">
+      <c r="AS1" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="AS1" s="36" t="s">
+      <c r="AT1" s="36" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -1746,34 +1749,107 @@
       <c r="AK2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="39" t="s">
+      <c r="AL2" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="AM2" s="39" t="s">
+      <c r="AN2" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="AN2" s="39">
+      <c r="AO2" s="39">
         <v>5000</v>
       </c>
-      <c r="AO2" s="39"/>
-      <c r="AQ2" s="40" t="s">
+      <c r="AP2" s="39"/>
+      <c r="AR2" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>193</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="AL3" s="39"/>
-      <c r="AM3" s="39"/>
-      <c r="AN3" s="39"/>
-      <c r="AO3" s="39"/>
+    <row r="3" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AE3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AJ3" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL3" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM3" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="AN3" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO3" s="39">
+        <v>5000</v>
+      </c>
       <c r="AP3" s="39"/>
-    </row>
-    <row r="4" spans="1:45" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR3" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>193</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1804,13 +1880,13 @@
       <c r="AC4" s="11"/>
       <c r="AE4" s="10"/>
       <c r="AH4" s="10"/>
-      <c r="AL4" s="39"/>
       <c r="AM4" s="39"/>
       <c r="AN4" s="39"/>
       <c r="AO4" s="39"/>
       <c r="AP4" s="39"/>
-    </row>
-    <row r="5" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ4" s="39"/>
+    </row>
+    <row r="5" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1841,13 +1917,13 @@
       <c r="AC5" s="11"/>
       <c r="AE5" s="10"/>
       <c r="AH5" s="10"/>
-      <c r="AL5" s="39"/>
       <c r="AM5" s="39"/>
       <c r="AN5" s="39"/>
       <c r="AO5" s="39"/>
       <c r="AP5" s="39"/>
-    </row>
-    <row r="6" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ5" s="39"/>
+    </row>
+    <row r="6" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1878,13 +1954,13 @@
       <c r="AC6" s="11"/>
       <c r="AE6" s="10"/>
       <c r="AH6" s="10"/>
-      <c r="AL6" s="39"/>
       <c r="AM6" s="39"/>
       <c r="AN6" s="39"/>
       <c r="AO6" s="39"/>
       <c r="AP6" s="39"/>
-    </row>
-    <row r="7" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ6" s="39"/>
+    </row>
+    <row r="7" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1915,13 +1991,13 @@
       <c r="AC7" s="11"/>
       <c r="AE7" s="10"/>
       <c r="AH7" s="10"/>
-      <c r="AL7" s="39"/>
       <c r="AM7" s="39"/>
       <c r="AN7" s="39"/>
       <c r="AO7" s="39"/>
       <c r="AP7" s="39"/>
-    </row>
-    <row r="8" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ7" s="39"/>
+    </row>
+    <row r="8" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1952,13 +2028,13 @@
       <c r="AC8" s="11"/>
       <c r="AE8" s="10"/>
       <c r="AH8" s="10"/>
-      <c r="AL8" s="39"/>
       <c r="AM8" s="39"/>
       <c r="AN8" s="39"/>
       <c r="AO8" s="39"/>
       <c r="AP8" s="39"/>
-    </row>
-    <row r="9" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ8" s="39"/>
+    </row>
+    <row r="9" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1989,13 +2065,13 @@
       <c r="AC9" s="11"/>
       <c r="AE9" s="10"/>
       <c r="AH9" s="10"/>
-      <c r="AL9" s="39"/>
       <c r="AM9" s="39"/>
       <c r="AN9" s="39"/>
       <c r="AO9" s="39"/>
       <c r="AP9" s="39"/>
-    </row>
-    <row r="10" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ9" s="39"/>
+    </row>
+    <row r="10" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -2026,13 +2102,13 @@
       <c r="AC10" s="11"/>
       <c r="AE10" s="10"/>
       <c r="AH10" s="10"/>
-      <c r="AL10" s="39"/>
       <c r="AM10" s="39"/>
       <c r="AN10" s="39"/>
       <c r="AO10" s="39"/>
       <c r="AP10" s="39"/>
-    </row>
-    <row r="11" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ10" s="39"/>
+    </row>
+    <row r="11" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -2063,13 +2139,13 @@
       <c r="AC11" s="11"/>
       <c r="AE11" s="10"/>
       <c r="AH11" s="10"/>
-      <c r="AL11" s="39"/>
       <c r="AM11" s="39"/>
       <c r="AN11" s="39"/>
       <c r="AO11" s="39"/>
       <c r="AP11" s="39"/>
-    </row>
-    <row r="12" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ11" s="39"/>
+    </row>
+    <row r="12" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2100,13 +2176,13 @@
       <c r="AC12" s="11"/>
       <c r="AE12" s="10"/>
       <c r="AH12" s="10"/>
-      <c r="AL12" s="39"/>
       <c r="AM12" s="39"/>
       <c r="AN12" s="39"/>
       <c r="AO12" s="39"/>
       <c r="AP12" s="39"/>
-    </row>
-    <row r="13" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ12" s="39"/>
+    </row>
+    <row r="13" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2137,13 +2213,13 @@
       <c r="AC13" s="11"/>
       <c r="AE13" s="10"/>
       <c r="AH13" s="10"/>
-      <c r="AL13" s="39"/>
       <c r="AM13" s="39"/>
       <c r="AN13" s="39"/>
       <c r="AO13" s="39"/>
       <c r="AP13" s="39"/>
-    </row>
-    <row r="14" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ13" s="39"/>
+    </row>
+    <row r="14" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2174,13 +2250,13 @@
       <c r="AC14" s="11"/>
       <c r="AE14" s="10"/>
       <c r="AH14" s="10"/>
-      <c r="AL14" s="39"/>
       <c r="AM14" s="39"/>
       <c r="AN14" s="39"/>
       <c r="AO14" s="39"/>
       <c r="AP14" s="39"/>
-    </row>
-    <row r="15" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AQ14" s="39"/>
+    </row>
+    <row r="15" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2211,12 +2287,12 @@
       <c r="AC15" s="11"/>
       <c r="AE15" s="10"/>
       <c r="AH15" s="10"/>
-      <c r="AL15" s="39"/>
       <c r="AM15" s="39"/>
       <c r="AN15" s="39"/>
       <c r="AO15" s="39"/>
-    </row>
-    <row r="16" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP15" s="39"/>
+    </row>
+    <row r="16" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2247,12 +2323,12 @@
       <c r="AC16" s="11"/>
       <c r="AE16" s="10"/>
       <c r="AH16" s="10"/>
-      <c r="AL16" s="39"/>
       <c r="AM16" s="39"/>
       <c r="AN16" s="39"/>
       <c r="AO16" s="39"/>
-    </row>
-    <row r="17" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP16" s="39"/>
+    </row>
+    <row r="17" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -2283,12 +2359,12 @@
       <c r="AC17" s="11"/>
       <c r="AE17" s="10"/>
       <c r="AH17" s="10"/>
-      <c r="AL17" s="39"/>
       <c r="AM17" s="39"/>
       <c r="AN17" s="39"/>
       <c r="AO17" s="39"/>
-    </row>
-    <row r="18" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP17" s="39"/>
+    </row>
+    <row r="18" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2319,12 +2395,12 @@
       <c r="AC18" s="11"/>
       <c r="AE18" s="10"/>
       <c r="AH18" s="10"/>
-      <c r="AL18" s="39"/>
       <c r="AM18" s="39"/>
       <c r="AN18" s="39"/>
       <c r="AO18" s="39"/>
-    </row>
-    <row r="19" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP18" s="39"/>
+    </row>
+    <row r="19" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2355,12 +2431,12 @@
       <c r="AC19" s="11"/>
       <c r="AE19" s="10"/>
       <c r="AH19" s="10"/>
-      <c r="AL19" s="39"/>
       <c r="AM19" s="39"/>
       <c r="AN19" s="39"/>
       <c r="AO19" s="39"/>
-    </row>
-    <row r="20" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP19" s="39"/>
+    </row>
+    <row r="20" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2391,12 +2467,12 @@
       <c r="AC20" s="11"/>
       <c r="AE20" s="10"/>
       <c r="AH20" s="10"/>
-      <c r="AL20" s="39"/>
       <c r="AM20" s="39"/>
       <c r="AN20" s="39"/>
       <c r="AO20" s="39"/>
-    </row>
-    <row r="21" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP20" s="39"/>
+    </row>
+    <row r="21" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2427,12 +2503,12 @@
       <c r="AC21" s="11"/>
       <c r="AE21" s="10"/>
       <c r="AH21" s="10"/>
-      <c r="AL21" s="39"/>
       <c r="AM21" s="39"/>
       <c r="AN21" s="39"/>
       <c r="AO21" s="39"/>
-    </row>
-    <row r="22" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP21" s="39"/>
+    </row>
+    <row r="22" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2463,12 +2539,12 @@
       <c r="AC22" s="11"/>
       <c r="AE22" s="10"/>
       <c r="AH22" s="10"/>
-      <c r="AL22" s="39"/>
       <c r="AM22" s="39"/>
       <c r="AN22" s="39"/>
       <c r="AO22" s="39"/>
-    </row>
-    <row r="23" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP22" s="39"/>
+    </row>
+    <row r="23" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -2499,12 +2575,12 @@
       <c r="AC23" s="11"/>
       <c r="AE23" s="10"/>
       <c r="AH23" s="10"/>
-      <c r="AL23" s="39"/>
       <c r="AM23" s="39"/>
       <c r="AN23" s="39"/>
       <c r="AO23" s="39"/>
-    </row>
-    <row r="24" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP23" s="39"/>
+    </row>
+    <row r="24" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2535,12 +2611,12 @@
       <c r="AC24" s="11"/>
       <c r="AE24" s="10"/>
       <c r="AH24" s="10"/>
-      <c r="AL24" s="39"/>
       <c r="AM24" s="39"/>
       <c r="AN24" s="39"/>
       <c r="AO24" s="39"/>
-    </row>
-    <row r="25" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP24" s="39"/>
+    </row>
+    <row r="25" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -2571,12 +2647,12 @@
       <c r="AC25" s="11"/>
       <c r="AE25" s="10"/>
       <c r="AH25" s="10"/>
-      <c r="AL25" s="39"/>
       <c r="AM25" s="39"/>
       <c r="AN25" s="39"/>
       <c r="AO25" s="39"/>
-    </row>
-    <row r="26" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP25" s="39"/>
+    </row>
+    <row r="26" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2606,12 +2682,12 @@
       <c r="AB26" s="11"/>
       <c r="AC26" s="11"/>
       <c r="AH26" s="10"/>
-      <c r="AL26" s="39"/>
       <c r="AM26" s="39"/>
       <c r="AN26" s="39"/>
       <c r="AO26" s="39"/>
-    </row>
-    <row r="27" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP26" s="39"/>
+    </row>
+    <row r="27" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -2641,12 +2717,12 @@
       <c r="AB27" s="11"/>
       <c r="AC27" s="11"/>
       <c r="AH27" s="10"/>
-      <c r="AL27" s="39"/>
       <c r="AM27" s="39"/>
       <c r="AN27" s="39"/>
       <c r="AO27" s="39"/>
-    </row>
-    <row r="28" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP27" s="39"/>
+    </row>
+    <row r="28" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -2676,12 +2752,12 @@
       <c r="AB28" s="11"/>
       <c r="AC28" s="11"/>
       <c r="AH28" s="10"/>
-      <c r="AL28" s="39"/>
       <c r="AM28" s="39"/>
       <c r="AN28" s="39"/>
       <c r="AO28" s="39"/>
-    </row>
-    <row r="29" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP28" s="39"/>
+    </row>
+    <row r="29" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -2711,12 +2787,12 @@
       <c r="AB29" s="11"/>
       <c r="AC29" s="11"/>
       <c r="AH29" s="10"/>
-      <c r="AL29" s="39"/>
       <c r="AM29" s="39"/>
       <c r="AN29" s="39"/>
       <c r="AO29" s="39"/>
-    </row>
-    <row r="30" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP29" s="39"/>
+    </row>
+    <row r="30" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2746,12 +2822,12 @@
       <c r="AB30" s="11"/>
       <c r="AC30" s="11"/>
       <c r="AH30" s="10"/>
-      <c r="AL30" s="39"/>
       <c r="AM30" s="39"/>
       <c r="AN30" s="39"/>
       <c r="AO30" s="39"/>
-    </row>
-    <row r="31" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP30" s="39"/>
+    </row>
+    <row r="31" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -2781,12 +2857,12 @@
       <c r="AB31" s="11"/>
       <c r="AC31" s="11"/>
       <c r="AH31" s="10"/>
-      <c r="AL31" s="39"/>
       <c r="AM31" s="39"/>
       <c r="AN31" s="39"/>
       <c r="AO31" s="39"/>
-    </row>
-    <row r="32" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP31" s="39"/>
+    </row>
+    <row r="32" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -2816,12 +2892,12 @@
       <c r="AB32" s="11"/>
       <c r="AC32" s="11"/>
       <c r="AH32" s="10"/>
-      <c r="AL32" s="39"/>
       <c r="AM32" s="39"/>
       <c r="AN32" s="39"/>
       <c r="AO32" s="39"/>
-    </row>
-    <row r="33" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP32" s="39"/>
+    </row>
+    <row r="33" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -2851,12 +2927,12 @@
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
       <c r="AH33" s="10"/>
-      <c r="AL33" s="39"/>
       <c r="AM33" s="39"/>
       <c r="AN33" s="39"/>
       <c r="AO33" s="39"/>
-    </row>
-    <row r="34" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP33" s="39"/>
+    </row>
+    <row r="34" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -2886,12 +2962,12 @@
       <c r="AB34" s="11"/>
       <c r="AC34" s="11"/>
       <c r="AH34" s="10"/>
-      <c r="AL34" s="39"/>
       <c r="AM34" s="39"/>
       <c r="AN34" s="39"/>
       <c r="AO34" s="39"/>
-    </row>
-    <row r="35" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP34" s="39"/>
+    </row>
+    <row r="35" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -2921,12 +2997,12 @@
       <c r="AB35" s="11"/>
       <c r="AC35" s="11"/>
       <c r="AH35" s="10"/>
-      <c r="AL35" s="39"/>
       <c r="AM35" s="39"/>
       <c r="AN35" s="39"/>
       <c r="AO35" s="39"/>
-    </row>
-    <row r="36" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP35" s="39"/>
+    </row>
+    <row r="36" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -2956,12 +3032,12 @@
       <c r="AB36" s="11"/>
       <c r="AC36" s="11"/>
       <c r="AH36" s="10"/>
-      <c r="AL36" s="39"/>
       <c r="AM36" s="39"/>
       <c r="AN36" s="39"/>
       <c r="AO36" s="39"/>
-    </row>
-    <row r="37" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP36" s="39"/>
+    </row>
+    <row r="37" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -2991,12 +3067,12 @@
       <c r="AB37" s="11"/>
       <c r="AC37" s="11"/>
       <c r="AH37" s="10"/>
-      <c r="AL37" s="39"/>
       <c r="AM37" s="39"/>
       <c r="AN37" s="39"/>
       <c r="AO37" s="39"/>
-    </row>
-    <row r="38" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP37" s="39"/>
+    </row>
+    <row r="38" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -3026,12 +3102,12 @@
       <c r="AB38" s="11"/>
       <c r="AC38" s="11"/>
       <c r="AH38" s="10"/>
-      <c r="AL38" s="39"/>
       <c r="AM38" s="39"/>
       <c r="AN38" s="39"/>
       <c r="AO38" s="39"/>
-    </row>
-    <row r="39" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP38" s="39"/>
+    </row>
+    <row r="39" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -3061,12 +3137,12 @@
       <c r="AB39" s="11"/>
       <c r="AC39" s="11"/>
       <c r="AH39" s="10"/>
-      <c r="AL39" s="39"/>
       <c r="AM39" s="39"/>
       <c r="AN39" s="39"/>
       <c r="AO39" s="39"/>
-    </row>
-    <row r="40" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP39" s="39"/>
+    </row>
+    <row r="40" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -3096,12 +3172,12 @@
       <c r="AB40" s="11"/>
       <c r="AC40" s="11"/>
       <c r="AH40" s="10"/>
-      <c r="AL40" s="39"/>
       <c r="AM40" s="39"/>
       <c r="AN40" s="39"/>
       <c r="AO40" s="39"/>
-    </row>
-    <row r="41" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP40" s="39"/>
+    </row>
+    <row r="41" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
@@ -3131,12 +3207,12 @@
       <c r="AB41" s="11"/>
       <c r="AC41" s="11"/>
       <c r="AH41" s="10"/>
-      <c r="AL41" s="39"/>
       <c r="AM41" s="39"/>
       <c r="AN41" s="39"/>
       <c r="AO41" s="39"/>
-    </row>
-    <row r="42" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP41" s="39"/>
+    </row>
+    <row r="42" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
@@ -3166,12 +3242,12 @@
       <c r="AB42" s="11"/>
       <c r="AC42" s="11"/>
       <c r="AH42" s="10"/>
-      <c r="AL42" s="39"/>
       <c r="AM42" s="39"/>
       <c r="AN42" s="39"/>
       <c r="AO42" s="39"/>
-    </row>
-    <row r="43" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP42" s="39"/>
+    </row>
+    <row r="43" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
@@ -3201,12 +3277,12 @@
       <c r="AB43" s="11"/>
       <c r="AC43" s="11"/>
       <c r="AH43" s="10"/>
-      <c r="AL43" s="39"/>
       <c r="AM43" s="39"/>
       <c r="AN43" s="39"/>
       <c r="AO43" s="39"/>
-    </row>
-    <row r="44" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP43" s="39"/>
+    </row>
+    <row r="44" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
@@ -3236,12 +3312,12 @@
       <c r="AB44" s="11"/>
       <c r="AC44" s="11"/>
       <c r="AH44" s="10"/>
-      <c r="AL44" s="39"/>
       <c r="AM44" s="39"/>
       <c r="AN44" s="39"/>
       <c r="AO44" s="39"/>
-    </row>
-    <row r="45" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP44" s="39"/>
+    </row>
+    <row r="45" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -3271,12 +3347,12 @@
       <c r="AB45" s="11"/>
       <c r="AC45" s="11"/>
       <c r="AH45" s="10"/>
-      <c r="AL45" s="39"/>
       <c r="AM45" s="39"/>
       <c r="AN45" s="39"/>
       <c r="AO45" s="39"/>
-    </row>
-    <row r="46" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP45" s="39"/>
+    </row>
+    <row r="46" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
@@ -3306,11 +3382,11 @@
       <c r="AB46" s="11"/>
       <c r="AC46" s="11"/>
       <c r="AH46" s="10"/>
-      <c r="AM46" s="39"/>
       <c r="AN46" s="39"/>
       <c r="AO46" s="39"/>
-    </row>
-    <row r="47" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP46" s="39"/>
+    </row>
+    <row r="47" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
@@ -3340,11 +3416,11 @@
       <c r="AB47" s="11"/>
       <c r="AC47" s="11"/>
       <c r="AH47" s="10"/>
-      <c r="AM47" s="39"/>
       <c r="AN47" s="39"/>
       <c r="AO47" s="39"/>
-    </row>
-    <row r="48" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP47" s="39"/>
+    </row>
+    <row r="48" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
@@ -3374,11 +3450,11 @@
       <c r="AB48" s="11"/>
       <c r="AC48" s="11"/>
       <c r="AH48" s="10"/>
-      <c r="AM48" s="39"/>
       <c r="AN48" s="39"/>
       <c r="AO48" s="39"/>
-    </row>
-    <row r="49" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP48" s="39"/>
+    </row>
+    <row r="49" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
@@ -3408,11 +3484,11 @@
       <c r="AB49" s="11"/>
       <c r="AC49" s="11"/>
       <c r="AH49" s="10"/>
-      <c r="AM49" s="39"/>
       <c r="AN49" s="39"/>
       <c r="AO49" s="39"/>
-    </row>
-    <row r="50" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP49" s="39"/>
+    </row>
+    <row r="50" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
@@ -3442,11 +3518,11 @@
       <c r="AB50" s="11"/>
       <c r="AC50" s="11"/>
       <c r="AH50" s="10"/>
-      <c r="AM50" s="39"/>
       <c r="AN50" s="39"/>
       <c r="AO50" s="39"/>
-    </row>
-    <row r="51" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP50" s="39"/>
+    </row>
+    <row r="51" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -3476,11 +3552,11 @@
       <c r="AB51" s="11"/>
       <c r="AC51" s="11"/>
       <c r="AH51" s="10"/>
-      <c r="AM51" s="39"/>
       <c r="AN51" s="39"/>
       <c r="AO51" s="39"/>
-    </row>
-    <row r="52" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP51" s="39"/>
+    </row>
+    <row r="52" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
@@ -3510,11 +3586,11 @@
       <c r="AB52" s="11"/>
       <c r="AC52" s="11"/>
       <c r="AH52" s="10"/>
-      <c r="AM52" s="39"/>
       <c r="AN52" s="39"/>
       <c r="AO52" s="39"/>
-    </row>
-    <row r="53" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP52" s="39"/>
+    </row>
+    <row r="53" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
@@ -3544,11 +3620,11 @@
       <c r="AB53" s="11"/>
       <c r="AC53" s="11"/>
       <c r="AH53" s="10"/>
-      <c r="AM53" s="39"/>
       <c r="AN53" s="39"/>
       <c r="AO53" s="39"/>
-    </row>
-    <row r="54" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP53" s="39"/>
+    </row>
+    <row r="54" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -3578,11 +3654,11 @@
       <c r="AB54" s="11"/>
       <c r="AC54" s="11"/>
       <c r="AH54" s="10"/>
-      <c r="AM54" s="39"/>
       <c r="AN54" s="39"/>
       <c r="AO54" s="39"/>
-    </row>
-    <row r="55" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP54" s="39"/>
+    </row>
+    <row r="55" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
@@ -3612,11 +3688,11 @@
       <c r="AB55" s="11"/>
       <c r="AC55" s="11"/>
       <c r="AH55" s="10"/>
-      <c r="AM55" s="39"/>
       <c r="AN55" s="39"/>
       <c r="AO55" s="39"/>
-    </row>
-    <row r="56" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP55" s="39"/>
+    </row>
+    <row r="56" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -3646,11 +3722,11 @@
       <c r="AB56" s="11"/>
       <c r="AC56" s="11"/>
       <c r="AH56" s="10"/>
-      <c r="AM56" s="39"/>
       <c r="AN56" s="39"/>
       <c r="AO56" s="39"/>
-    </row>
-    <row r="57" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP56" s="39"/>
+    </row>
+    <row r="57" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -3680,11 +3756,11 @@
       <c r="AB57" s="11"/>
       <c r="AC57" s="11"/>
       <c r="AH57" s="10"/>
-      <c r="AM57" s="39"/>
       <c r="AN57" s="39"/>
       <c r="AO57" s="39"/>
-    </row>
-    <row r="58" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP57" s="39"/>
+    </row>
+    <row r="58" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -3714,11 +3790,11 @@
       <c r="AB58" s="11"/>
       <c r="AC58" s="11"/>
       <c r="AH58" s="10"/>
-      <c r="AM58" s="39"/>
       <c r="AN58" s="39"/>
       <c r="AO58" s="39"/>
-    </row>
-    <row r="59" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP58" s="39"/>
+    </row>
+    <row r="59" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -3748,11 +3824,11 @@
       <c r="AB59" s="11"/>
       <c r="AC59" s="11"/>
       <c r="AH59" s="10"/>
-      <c r="AM59" s="39"/>
       <c r="AN59" s="39"/>
       <c r="AO59" s="39"/>
-    </row>
-    <row r="60" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP59" s="39"/>
+    </row>
+    <row r="60" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -3782,11 +3858,11 @@
       <c r="AB60" s="11"/>
       <c r="AC60" s="11"/>
       <c r="AH60" s="10"/>
-      <c r="AM60" s="39"/>
       <c r="AN60" s="39"/>
       <c r="AO60" s="39"/>
-    </row>
-    <row r="61" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP60" s="39"/>
+    </row>
+    <row r="61" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -3816,11 +3892,11 @@
       <c r="AB61" s="11"/>
       <c r="AC61" s="11"/>
       <c r="AH61" s="10"/>
-      <c r="AM61" s="39"/>
       <c r="AN61" s="39"/>
       <c r="AO61" s="39"/>
-    </row>
-    <row r="62" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP61" s="39"/>
+    </row>
+    <row r="62" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -3850,11 +3926,11 @@
       <c r="AB62" s="11"/>
       <c r="AC62" s="11"/>
       <c r="AH62" s="10"/>
-      <c r="AM62" s="39"/>
       <c r="AN62" s="39"/>
       <c r="AO62" s="39"/>
-    </row>
-    <row r="63" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP62" s="39"/>
+    </row>
+    <row r="63" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="10"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -3884,11 +3960,11 @@
       <c r="AB63" s="11"/>
       <c r="AC63" s="11"/>
       <c r="AH63" s="10"/>
-      <c r="AM63" s="39"/>
       <c r="AN63" s="39"/>
       <c r="AO63" s="39"/>
-    </row>
-    <row r="64" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP63" s="39"/>
+    </row>
+    <row r="64" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -3918,11 +3994,11 @@
       <c r="AB64" s="11"/>
       <c r="AC64" s="11"/>
       <c r="AH64" s="10"/>
-      <c r="AM64" s="39"/>
       <c r="AN64" s="39"/>
       <c r="AO64" s="39"/>
-    </row>
-    <row r="65" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP64" s="39"/>
+    </row>
+    <row r="65" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
@@ -3952,11 +4028,11 @@
       <c r="AB65" s="11"/>
       <c r="AC65" s="11"/>
       <c r="AH65" s="10"/>
-      <c r="AM65" s="39"/>
       <c r="AN65" s="39"/>
       <c r="AO65" s="39"/>
-    </row>
-    <row r="66" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP65" s="39"/>
+    </row>
+    <row r="66" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -3986,11 +4062,11 @@
       <c r="AB66" s="11"/>
       <c r="AC66" s="11"/>
       <c r="AH66" s="10"/>
-      <c r="AM66" s="39"/>
       <c r="AN66" s="39"/>
       <c r="AO66" s="39"/>
-    </row>
-    <row r="67" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP66" s="39"/>
+    </row>
+    <row r="67" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -4020,11 +4096,11 @@
       <c r="AB67" s="11"/>
       <c r="AC67" s="11"/>
       <c r="AH67" s="10"/>
-      <c r="AM67" s="39"/>
       <c r="AN67" s="39"/>
       <c r="AO67" s="39"/>
-    </row>
-    <row r="68" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP67" s="39"/>
+    </row>
+    <row r="68" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -4053,11 +4129,11 @@
       <c r="AA68" s="11"/>
       <c r="AB68" s="11"/>
       <c r="AC68" s="11"/>
-      <c r="AM68" s="39"/>
       <c r="AN68" s="39"/>
       <c r="AO68" s="39"/>
-    </row>
-    <row r="69" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP68" s="39"/>
+    </row>
+    <row r="69" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
@@ -4086,11 +4162,11 @@
       <c r="AA69" s="11"/>
       <c r="AB69" s="11"/>
       <c r="AC69" s="11"/>
-      <c r="AM69" s="39"/>
       <c r="AN69" s="39"/>
       <c r="AO69" s="39"/>
-    </row>
-    <row r="70" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP69" s="39"/>
+    </row>
+    <row r="70" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
@@ -4119,11 +4195,11 @@
       <c r="AA70" s="11"/>
       <c r="AB70" s="11"/>
       <c r="AC70" s="11"/>
-      <c r="AM70" s="39"/>
       <c r="AN70" s="39"/>
       <c r="AO70" s="39"/>
-    </row>
-    <row r="71" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AP70" s="39"/>
+    </row>
+    <row r="71" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -4152,11 +4228,11 @@
       <c r="AA71" s="11"/>
       <c r="AB71" s="11"/>
       <c r="AC71" s="11"/>
-      <c r="AM71" s="39"/>
       <c r="AN71" s="39"/>
       <c r="AO71" s="39"/>
-    </row>
-    <row r="72" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="AP71" s="39"/>
+    </row>
+    <row r="72" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -4186,7 +4262,7 @@
       <c r="AB72" s="11"/>
       <c r="AC72" s="11"/>
     </row>
-    <row r="73" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
@@ -4216,7 +4292,7 @@
       <c r="AB73" s="11"/>
       <c r="AC73" s="11"/>
     </row>
-    <row r="74" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
@@ -4246,7 +4322,7 @@
       <c r="AB74" s="11"/>
       <c r="AC74" s="11"/>
     </row>
-    <row r="75" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -4276,7 +4352,7 @@
       <c r="AB75" s="11"/>
       <c r="AC75" s="11"/>
     </row>
-    <row r="76" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -4306,7 +4382,7 @@
       <c r="AB76" s="11"/>
       <c r="AC76" s="11"/>
     </row>
-    <row r="77" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -4336,7 +4412,7 @@
       <c r="AB77" s="11"/>
       <c r="AC77" s="11"/>
     </row>
-    <row r="78" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -4366,7 +4442,7 @@
       <c r="AB78" s="11"/>
       <c r="AC78" s="11"/>
     </row>
-    <row r="79" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B79" s="10"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -4396,7 +4472,7 @@
       <c r="AB79" s="11"/>
       <c r="AC79" s="11"/>
     </row>
-    <row r="80" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B80" s="10"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -6438,26 +6514,26 @@
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="AQ1:AS1 AQ4:AS14 AP15:AS71 A72:AS147 A1:AO2 AQ2 AP3:AP14 AL3:AL45 AM3:AO71 A4:AK45 A46:AL71">
+  <conditionalFormatting sqref="AR1:AT1 A4:AT147 AR2:AR3 A1:AP3">
     <cfRule type="expression" dxfId="9" priority="3">
       <formula>ISNUMBER(SEARCH("FAIL", $A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR1 AR3:AR1048576">
+  <conditionalFormatting sqref="AS1 AS4:AS1048576">
     <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",AR1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",AS1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR1 AR4:AR1048576">
+  <conditionalFormatting sqref="AS1 AS4:AS1048576">
     <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",AR1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",AS1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 J2 J4:J25 G2 G4:G25 AE2 AE4:AE25 AH2 AH4:AH67 AK2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3 J2:J25 G2:G25 AE2:AE25 AH2:AH67 AK2:AK3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Bao gồm,Loại trừ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Loại trừ,Cộng dồn,Bậc thang"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6477,18 +6553,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="46" width="5.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="46" width="18.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="46" width="8.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="46" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="46" width="14.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="46" width="18.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="47" width="18.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="47" width="26.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="47" width="28.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="46" width="37.21875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="46" width="36.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="1" max="1" width="5.77734375" style="46" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.5546875" style="46" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.88671875" style="46" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.44140625" style="46" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" style="46" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.21875" style="46" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.21875" style="47" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.109375" style="47" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.77734375" style="47" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="37.21875" style="46" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.44140625" style="46" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="42" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -7280,14 +7356,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
@@ -7579,22 +7655,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG61"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView showFormulas="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="24" width="10.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="24" width="6.88671875" collapsed="true"/>
-    <col min="13" max="17" style="24" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="10.21875" style="24" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.88671875" style="24" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="8.88671875" style="24" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -7680,10 +7756,10 @@
       <c r="L4" s="27"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
     </row>
@@ -7694,7 +7770,7 @@
       <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="50">
         <v>2</v>
       </c>
       <c r="E9" s="14">
@@ -7707,7 +7783,7 @@
       <c r="B10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="50"/>
       <c r="E10" s="14">
         <v>2</v>
       </c>
@@ -7735,7 +7811,7 @@
       <c r="B12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="50">
         <v>2</v>
       </c>
       <c r="E12" s="14">
@@ -7748,7 +7824,7 @@
       <c r="B13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="53"/>
+      <c r="C13" s="50"/>
       <c r="E13" s="14">
         <v>5</v>
       </c>
@@ -7761,7 +7837,7 @@
       <c r="B14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="51">
         <v>2</v>
       </c>
       <c r="E14" s="14">
@@ -7774,7 +7850,7 @@
       <c r="B15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="50"/>
+      <c r="C15" s="52"/>
       <c r="E15" s="14">
         <v>7</v>
       </c>
@@ -7787,7 +7863,7 @@
       <c r="B16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="51">
         <v>2</v>
       </c>
       <c r="E16" s="14">
@@ -7800,7 +7876,7 @@
       <c r="B17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="52"/>
       <c r="E17" s="14">
         <v>9</v>
       </c>
@@ -7813,7 +7889,7 @@
       <c r="B18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="51">
         <v>2</v>
       </c>
       <c r="E18" s="14">
@@ -7826,7 +7902,7 @@
       <c r="B19" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="52"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -8533,22 +8609,22 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="51" t="s">
         <v>20</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="53">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="53"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
@@ -8562,40 +8638,40 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="51" t="s">
         <v>80</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="51">
+      <c r="C40" s="53">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="50"/>
+      <c r="A41" s="52"/>
       <c r="B41" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="51"/>
+      <c r="C41" s="53"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="51" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="51">
+      <c r="C42" s="53">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="50"/>
+      <c r="A43" s="52"/>
       <c r="B43" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="51"/>
+      <c r="C43" s="53"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C44">
@@ -8874,11 +8950,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A40:A41"/>
@@ -8886,6 +8957,11 @@
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8903,11 +8979,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.77734375" collapsed="true"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -9055,35 +9131,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="19" width="4.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="15" width="13.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="16" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="16" width="13.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="8" width="17.77734375" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" style="15" width="19.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="16" width="21.77734375" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="16" width="18.21875" collapsed="true"/>
-    <col min="12" max="14" customWidth="true" style="17" width="18.77734375" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="18" max="20" customWidth="true" style="15" width="17.0" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="24" max="26" customWidth="true" style="15" width="17.0" collapsed="true"/>
-    <col min="27" max="29" customWidth="true" style="16" width="17.0" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="37" width="25.6640625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="37" width="17.0" collapsed="true"/>
-    <col min="32" max="34" customWidth="true" style="19" width="17.0" collapsed="true"/>
-    <col min="35" max="36" customWidth="true" style="37" width="17.0" collapsed="true"/>
-    <col min="37" max="40" customWidth="true" style="37" width="16.88671875" collapsed="true"/>
-    <col min="41" max="42" customWidth="true" style="37" width="15.109375" collapsed="true"/>
-    <col min="43" max="43" customWidth="true" style="37" width="16.21875" collapsed="true"/>
-    <col min="44" max="44" customWidth="true" style="19" width="32.6640625" collapsed="true"/>
-    <col min="45" max="46" customWidth="true" style="19" width="19.21875" collapsed="true"/>
-    <col min="47" max="47" style="37" width="8.88671875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="37" width="13.0" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" style="37" width="11.6640625" collapsed="true"/>
-    <col min="50" max="58" style="37" width="8.88671875" collapsed="true"/>
-    <col min="59" max="59" customWidth="true" style="14" width="35.5546875" collapsed="true"/>
-    <col min="60" max="16384" style="14" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="4.33203125" style="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.77734375" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.77734375" style="8" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.77734375" style="16" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="18.21875" style="16" customWidth="1" collapsed="1"/>
+    <col min="12" max="14" width="18.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="18" max="20" width="17" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="24" max="26" width="17" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="29" width="17" style="16" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="25.6640625" style="37" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="17" style="37" customWidth="1" collapsed="1"/>
+    <col min="32" max="34" width="17" style="19" customWidth="1" collapsed="1"/>
+    <col min="35" max="36" width="17" style="37" customWidth="1" collapsed="1"/>
+    <col min="37" max="40" width="16.88671875" style="37" customWidth="1" collapsed="1"/>
+    <col min="41" max="42" width="15.109375" style="37" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="16.21875" style="37" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="32.6640625" style="19" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="19.21875" style="19" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="8.88671875" style="37" collapsed="1"/>
+    <col min="48" max="48" width="13" style="37" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.6640625" style="37" customWidth="1" collapsed="1"/>
+    <col min="50" max="58" width="8.88671875" style="37" collapsed="1"/>
+    <col min="59" max="59" width="35.5546875" style="14" customWidth="1" collapsed="1"/>
+    <col min="60" max="16384" width="8.88671875" style="14" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" s="36" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update code hình thwucs giảm giá sp theo bội sô
</commit_message>
<xml_diff>
--- a/src/main/resources/HTGiamGiaSPTheoBoiSo.xlsx
+++ b/src/main/resources/HTGiamGiaSPTheoBoiSo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThuPhuoc\MyAutomation\finviet\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Auto_Company\FinViet2024\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA2C8C7-C4B0-4668-9200-84B259FC6DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="12240" tabRatio="580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="12240" tabRatio="580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ThongTinCoBanKM" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Infor" sheetId="8" r:id="rId6"/>
     <sheet name="copy" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="189">
   <si>
     <t>Kênh mua hàng</t>
   </si>
@@ -546,15 +545,6 @@
     <t>promotions_allow_apply.id</t>
   </si>
   <si>
-    <t>0968686868,0368199222</t>
-  </si>
-  <si>
-    <t>Quantity_Mong đợi</t>
-  </si>
-  <si>
-    <t>Quantity_Thực tế</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
@@ -564,36 +554,15 @@
     <t>SchemaID_Mong đợi</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Name_Mong đợi</t>
   </si>
   <si>
     <t>Name_Thực tế</t>
   </si>
   <si>
-    <t>Auto_KM_27/06/2024 08:31</t>
-  </si>
-  <si>
-    <t>Auto_KM_27/06/2024 08:33</t>
-  </si>
-  <si>
-    <t>Auto_KM_27/06/2024 08:35</t>
-  </si>
-  <si>
     <t>SchemaName</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>Danh sách sản phẩm của NPP</t>
   </si>
   <si>
@@ -621,16 +590,28 @@
     <t>Giá trị giảm_Giảm số tiền cố định</t>
   </si>
   <si>
-    <t>c2acc717-daa5-4929-a22e-c789057d9b27</t>
-  </si>
-  <si>
-    <t>Auto_KM_GiamGiaSPTheoBoiSo04/07/2024 15:05</t>
+    <t>GiaSPSauKM_Thực tế</t>
+  </si>
+  <si>
+    <t>GiaSPSauKM_Mong đợi</t>
+  </si>
+  <si>
+    <t>eb993bb1-67de-4331-ab04-df96650cf0ef</t>
+  </si>
+  <si>
+    <t>Auto_KM_GiamGiaSPTheoBoiSo05/07/2024 09:22</t>
+  </si>
+  <si>
+    <t>188750</t>
+  </si>
+  <si>
+    <t>189167</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,7 +975,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Style 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Style 1" xfId="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1401,7 +1382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1502,7 +1483,7 @@
     </row>
   </sheetData>
   <dataValidations xWindow="272" yWindow="419" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1512,13 +1493,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AT147"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
       <selection activeCell="BG2" sqref="BG2"/>
-      <selection pane="topRight" activeCell="AJ9" sqref="AJ9"/>
+      <selection pane="topRight" activeCell="AS14" sqref="AS14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,13 +1530,14 @@
     <col min="39" max="39" width="37.77734375" style="19" customWidth="1" collapsed="1"/>
     <col min="40" max="40" width="24.77734375" style="19" customWidth="1" collapsed="1"/>
     <col min="41" max="43" width="19.21875" style="19" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="25.77734375" style="19" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="35.5546875" style="14" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="23.88671875" style="14" customWidth="1" collapsed="1"/>
-    <col min="47" max="16384" width="8.88671875" style="14" collapsed="1"/>
+    <col min="44" max="44" width="35.5546875" style="14" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="23.88671875" style="14" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="8.88671875" style="14" collapsed="1"/>
+    <col min="47" max="47" width="8.88671875" style="14"/>
+    <col min="48" max="16384" width="8.88671875" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="36" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" s="36" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>69</v>
       </c>
@@ -1590,10 +1572,10 @@
         <v>59</v>
       </c>
       <c r="L1" s="48" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="N1" s="34" t="s">
         <v>55</v>
@@ -1671,31 +1653,28 @@
         <v>65</v>
       </c>
       <c r="AM1" s="29" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="AN1" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AO1" s="29" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="AP1" s="29" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AQ1" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="AR1" s="29" t="s">
-        <v>65</v>
+        <v>181</v>
+      </c>
+      <c r="AR1" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="AS1" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT1" s="36" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -1712,13 +1691,13 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="12" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="M2" s="12" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -1753,103 +1732,60 @@
         <v>64</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="AN2" s="39" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="AO2" s="39">
         <v>5000</v>
       </c>
       <c r="AP2" s="39"/>
-      <c r="AR2" s="40" t="s">
-        <v>168</v>
+      <c r="AR2" t="s">
+        <v>185</v>
       </c>
       <c r="AS2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>47</v>
-      </c>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>185</v>
-      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="13"/>
+      <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
-      <c r="X3" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z3" s="10">
-        <v>4</v>
-      </c>
-      <c r="AA3" s="13"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="11"/>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
       <c r="AE3" s="10"/>
       <c r="AH3" s="10"/>
-      <c r="AJ3" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL3" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM3" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="AN3" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="AO3" s="39">
-        <v>5000</v>
-      </c>
+      <c r="AM3" s="39"/>
+      <c r="AN3" s="39"/>
+      <c r="AO3" s="39"/>
       <c r="AP3" s="39"/>
-      <c r="AR3" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ3" s="39"/>
+    </row>
+    <row r="4" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1886,7 +1822,7 @@
       <c r="AP4" s="39"/>
       <c r="AQ4" s="39"/>
     </row>
-    <row r="5" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1923,7 +1859,7 @@
       <c r="AP5" s="39"/>
       <c r="AQ5" s="39"/>
     </row>
-    <row r="6" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1960,7 +1896,7 @@
       <c r="AP6" s="39"/>
       <c r="AQ6" s="39"/>
     </row>
-    <row r="7" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1997,7 +1933,7 @@
       <c r="AP7" s="39"/>
       <c r="AQ7" s="39"/>
     </row>
-    <row r="8" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -2034,7 +1970,7 @@
       <c r="AP8" s="39"/>
       <c r="AQ8" s="39"/>
     </row>
-    <row r="9" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -2071,7 +2007,7 @@
       <c r="AP9" s="39"/>
       <c r="AQ9" s="39"/>
     </row>
-    <row r="10" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -2108,7 +2044,7 @@
       <c r="AP10" s="39"/>
       <c r="AQ10" s="39"/>
     </row>
-    <row r="11" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -2145,7 +2081,7 @@
       <c r="AP11" s="39"/>
       <c r="AQ11" s="39"/>
     </row>
-    <row r="12" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2182,7 +2118,7 @@
       <c r="AP12" s="39"/>
       <c r="AQ12" s="39"/>
     </row>
-    <row r="13" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2219,7 +2155,7 @@
       <c r="AP13" s="39"/>
       <c r="AQ13" s="39"/>
     </row>
-    <row r="14" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2254,9 +2190,8 @@
       <c r="AN14" s="39"/>
       <c r="AO14" s="39"/>
       <c r="AP14" s="39"/>
-      <c r="AQ14" s="39"/>
-    </row>
-    <row r="15" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2292,7 +2227,7 @@
       <c r="AO15" s="39"/>
       <c r="AP15" s="39"/>
     </row>
-    <row r="16" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2639,13 +2574,12 @@
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
-      <c r="X25" s="18"/>
+      <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
       <c r="AC25" s="11"/>
-      <c r="AE25" s="10"/>
       <c r="AH25" s="10"/>
       <c r="AM25" s="39"/>
       <c r="AN25" s="39"/>
@@ -3347,7 +3281,6 @@
       <c r="AB45" s="11"/>
       <c r="AC45" s="11"/>
       <c r="AH45" s="10"/>
-      <c r="AM45" s="39"/>
       <c r="AN45" s="39"/>
       <c r="AO45" s="39"/>
       <c r="AP45" s="39"/>
@@ -4095,7 +4028,6 @@
       <c r="AA67" s="11"/>
       <c r="AB67" s="11"/>
       <c r="AC67" s="11"/>
-      <c r="AH67" s="10"/>
       <c r="AN67" s="39"/>
       <c r="AO67" s="39"/>
       <c r="AP67" s="39"/>
@@ -4199,7 +4131,7 @@
       <c r="AO70" s="39"/>
       <c r="AP70" s="39"/>
     </row>
-    <row r="71" spans="2:42" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -4228,9 +4160,6 @@
       <c r="AA71" s="11"/>
       <c r="AB71" s="11"/>
       <c r="AC71" s="11"/>
-      <c r="AN71" s="39"/>
-      <c r="AO71" s="39"/>
-      <c r="AP71" s="39"/>
     </row>
     <row r="72" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B72" s="10"/>
@@ -6482,58 +6411,28 @@
       <c r="AB146" s="11"/>
       <c r="AC146" s="11"/>
     </row>
-    <row r="147" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B147" s="10"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="10"/>
-      <c r="G147" s="10"/>
-      <c r="H147" s="10"/>
-      <c r="I147" s="11"/>
-      <c r="J147" s="11"/>
-      <c r="K147" s="11"/>
-      <c r="L147" s="12"/>
-      <c r="M147" s="12"/>
-      <c r="N147" s="12"/>
-      <c r="O147" s="11"/>
-      <c r="P147" s="11"/>
-      <c r="Q147" s="11"/>
-      <c r="R147" s="10"/>
-      <c r="S147" s="10"/>
-      <c r="T147" s="10"/>
-      <c r="U147" s="11"/>
-      <c r="V147" s="11"/>
-      <c r="W147" s="11"/>
-      <c r="X147" s="10"/>
-      <c r="Y147" s="10"/>
-      <c r="Z147" s="10"/>
-      <c r="AA147" s="11"/>
-      <c r="AB147" s="11"/>
-      <c r="AC147" s="11"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="AR1:AT1 A4:AT147 AR2:AR3 A1:AP3">
+  <conditionalFormatting sqref="AR1:AS1 A3:AS146 A1:AP2">
     <cfRule type="expression" dxfId="9" priority="3">
       <formula>ISNUMBER(SEARCH("FAIL", $A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS1 AS4:AS1048576">
+  <conditionalFormatting sqref="AR1 AR3:AR1048576">
     <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",AS1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",AR1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS1 AS4:AS1048576">
+  <conditionalFormatting sqref="AR1 AR3:AR1048576">
     <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",AS1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",AR1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3 J2:J25 G2:G25 AE2:AE25 AH2:AH67 AK2:AK3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 AK2 AH2:AH66 AE2:AE24 G2:G24 J2:J24">
       <formula1>"Bao gồm,Loại trừ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"Loại trừ,Cộng dồn,Bậc thang"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6543,12 +6442,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6584,22 +6483,22 @@
         <v>73</v>
       </c>
       <c r="F1" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="K1" s="43" t="s">
         <v>170</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>173</v>
       </c>
       <c r="L1" s="43" t="s">
         <v>76</v>
@@ -6621,16 +6520,31 @@
       <c r="E2" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="45">
-        <v>2</v>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K2" t="s">
+        <v>185</v>
       </c>
       <c r="L2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>86</v>
@@ -6642,185 +6556,69 @@
         <v>617895</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="45">
-        <v>4</v>
+        <v>64</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="G3" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="I3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="K3" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="L3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="46">
-        <v>3</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="46">
-        <v>6</v>
-      </c>
-      <c r="D4" s="46">
-        <v>616747</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="45">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>174</v>
-      </c>
-      <c r="H4" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L4" t="s">
-        <v>166</v>
-      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="46">
-        <v>4</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="46">
-        <v>4</v>
-      </c>
-      <c r="D5" s="46">
-        <v>616747</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="45">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" t="s">
-        <v>181</v>
-      </c>
-      <c r="I5" t="s">
-        <v>181</v>
-      </c>
-      <c r="J5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K5" t="s">
-        <v>153</v>
-      </c>
-      <c r="L5" t="s">
-        <v>171</v>
-      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="46">
-        <v>4</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="46">
-        <v>12</v>
-      </c>
-      <c r="D6" s="46">
-        <v>616747</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="45">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" t="s">
-        <v>181</v>
-      </c>
-      <c r="J6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L6" t="s">
-        <v>166</v>
-      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="46">
-        <v>4</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="46">
-        <v>2</v>
-      </c>
-      <c r="D7" s="46">
-        <v>616747</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="45">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L7" t="s">
-        <v>171</v>
+      <c r="L7" t="str">
+        <f t="shared" ref="L7:L38" si="0">IF(A7 &lt;&gt;"",IF(AND(J7=K7,J7&lt;&gt;"",K7&lt;&gt;""),"PASS","FAIL"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L11" t="str">
-        <f t="shared" ref="L11:L42" si="0">IF(A11 &lt;&gt;"",IF(AND(J11=K11,J11&lt;&gt;"",K11&lt;&gt;""),"PASS","FAIL"),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6988,31 +6786,31 @@
     </row>
     <row r="39" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L39:L70" si="1">IF(A39 &lt;&gt;"",IF(AND(J39=K39,J39&lt;&gt;"",K39&lt;&gt;""),"PASS","FAIL"),"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L43" t="str">
-        <f t="shared" ref="L43:L74" si="1">IF(A43 &lt;&gt;"",IF(AND(J43=K43,J43&lt;&gt;"",K43&lt;&gt;""),"PASS","FAIL"),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -7180,31 +6978,31 @@
     </row>
     <row r="71" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L71:L92" si="2">IF(A71 &lt;&gt;"",IF(AND(J71=K71,J71&lt;&gt;"",K71&lt;&gt;""),"PASS","FAIL"),"")</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L75" t="str">
-        <f t="shared" ref="L75:L96" si="2">IF(A75 &lt;&gt;"",IF(AND(J75=K75,J75&lt;&gt;"",K75&lt;&gt;""),"PASS","FAIL"),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -7306,30 +7104,6 @@
     </row>
     <row r="92" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L92" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L93" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L94" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L95" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L96" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -7347,7 +7121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
@@ -7383,10 +7157,10 @@
         <v>73</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>76</v>
@@ -7634,7 +7408,7 @@
         <v>153</v>
       </c>
       <c r="H11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -7652,7 +7426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG61"/>
   <sheetViews>
     <sheetView showFormulas="1" topLeftCell="A37" workbookViewId="0">
@@ -8970,11 +8744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9120,7 +8894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG155"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -14414,10 +14188,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J33 G2:G33 AS2:AS11 AM2:AM33 AP2:AP75" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J33 G2:G33 AS2:AS11 AM2:AM33 AP2:AP75">
       <formula1>"Bao gồm,Loại trừ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9">
       <formula1>"Loại trừ,Cộng dồn,Bậc thang"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>